<commit_message>
def update for Total Time (Minutes)
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/SurveyResults/Exploratory Delegation Variables.xlsx
+++ b/dashboard-ui/src/components/SurveyResults/Exploratory Delegation Variables.xlsx
@@ -31,7 +31,7 @@
     <t>End Time</t>
   </si>
   <si>
-    <t>Total Time</t>
+    <t>Total Time (Minutes)</t>
   </si>
   <si>
     <t>Post-Scenario Measures - Time Taken (Minutes)</t>
@@ -967,7 +967,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -978,12 +978,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1015,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1023,17 +1017,11 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1343,46 +1331,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="5" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="5" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="5" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="5" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="5" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="5" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="5" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="5" width="22.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="5" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="5" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="5" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="6" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="5" width="25.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="4" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="4" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="4" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="4" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="4" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="4" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="4" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="4" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="4" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="4" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="4" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="4" width="25.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="51" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="60" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1446,10 +1434,10 @@
       <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="X1" s="2" t="s">
@@ -1473,10 +1461,10 @@
       <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
       <c r="AG1" s="2" t="s">
@@ -1488,14 +1476,14 @@
       <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="208.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="249" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1559,10 +1547,10 @@
       <c r="U2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>59</v>
       </c>
       <c r="X2" s="2" t="s">
@@ -1586,10 +1574,10 @@
       <c r="AD2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AE2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" s="2" t="s">
         <v>68</v>
       </c>
       <c r="AG2" s="2" t="s">
@@ -1601,10 +1589,10 @@
       <c r="AI2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK2" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1617,7 +1605,7 @@
         <v>74</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
@@ -1656,10 +1644,10 @@
       <c r="U3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="2" t="s">
         <v>86</v>
       </c>
       <c r="X3" s="2"/>
@@ -1671,8 +1659,8 @@
         <v>87</v>
       </c>
       <c r="AD3" s="2"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2" t="s">
         <v>88</v>
@@ -1680,10 +1668,10 @@
       <c r="AI3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AJ3" s="3" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AK3" s="2" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>